<commit_message>
add UN population and fertility estimates
</commit_message>
<xml_diff>
--- a/Config/Kenya_parameters.xlsx
+++ b/Config/Kenya_parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17925" windowHeight="9000" tabRatio="641" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" tabRatio="641" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="10" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2455" uniqueCount="1082">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="1086">
   <si>
     <t>Metric</t>
   </si>
@@ -3298,12 +3298,24 @@
   <si>
     <t>Births per 1000 women</t>
   </si>
+  <si>
+    <t>Source: UN Department of Economic and Social Affairs: World Population Prospects 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Males </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Females </t>
+  </si>
+  <si>
+    <t>HIV negative</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="9">
+  <numFmts count="11">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
@@ -3313,6 +3325,8 @@
     <numFmt numFmtId="170" formatCode="0.0000"/>
     <numFmt numFmtId="171" formatCode="#,##0.000"/>
     <numFmt numFmtId="172" formatCode="##0.0;\-##0.0;0"/>
+    <numFmt numFmtId="173" formatCode="#\ ###\ ###\ ##0;\-#\ ###\ ###\ ##0;0"/>
+    <numFmt numFmtId="176" formatCode="##0.0000;\-##0.0000;0.000"/>
   </numFmts>
   <fonts count="27" x14ac:knownFonts="1">
     <font>
@@ -3924,7 +3938,7 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3978,9 +3992,6 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="23" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3991,6 +4002,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="172" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -6313,6 +6334,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7419,6 +7441,7 @@
         <c:idx val="3"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7533,6 +7556,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8580,6 +8604,7 @@
         <c:idx val="3"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8686,6 +8711,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9637,6 +9663,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19705,10 +19732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y117"/>
+  <dimension ref="A1:Y168"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="J85" sqref="J85"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U147" sqref="U147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24057,7 +24084,7 @@
         <v>38610097</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>699</v>
       </c>
@@ -24080,7 +24107,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="114" spans="1:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B114" s="37">
         <v>1979</v>
       </c>
@@ -24105,7 +24132,7 @@
         <v>7706115</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B115">
         <v>1989</v>
       </c>
@@ -24130,7 +24157,7 @@
         <v>5704992</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B116">
         <v>1999</v>
       </c>
@@ -24155,7 +24182,7 @@
         <v>8184885</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B117">
         <v>2009</v>
       </c>
@@ -24179,6 +24206,1913 @@
         <f>SUM(H94:H107)</f>
         <v>11234575</v>
       </c>
+    </row>
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C126" s="47">
+        <v>1950</v>
+      </c>
+      <c r="D126" s="47">
+        <v>1955</v>
+      </c>
+      <c r="E126" s="47">
+        <v>1960</v>
+      </c>
+      <c r="F126" s="47">
+        <v>1965</v>
+      </c>
+      <c r="G126" s="47">
+        <v>1970</v>
+      </c>
+      <c r="H126" s="47">
+        <v>1975</v>
+      </c>
+      <c r="I126" s="47">
+        <v>1980</v>
+      </c>
+      <c r="J126" s="47">
+        <v>1985</v>
+      </c>
+      <c r="K126" s="47">
+        <v>1990</v>
+      </c>
+      <c r="L126" s="47">
+        <v>1995</v>
+      </c>
+      <c r="M126" s="47">
+        <v>2000</v>
+      </c>
+      <c r="N126" s="47">
+        <v>2005</v>
+      </c>
+      <c r="O126" s="47">
+        <v>2010</v>
+      </c>
+      <c r="P126" s="47">
+        <v>2015</v>
+      </c>
+      <c r="Q126" s="47">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B127" s="46" t="s">
+        <v>499</v>
+      </c>
+      <c r="C127" s="50">
+        <v>530.10400000000004</v>
+      </c>
+      <c r="D127" s="50">
+        <v>677.54600000000005</v>
+      </c>
+      <c r="E127" s="50">
+        <v>801.89499999999998</v>
+      </c>
+      <c r="F127" s="50">
+        <v>952.15599999999995</v>
+      </c>
+      <c r="G127" s="50">
+        <v>1142.9079999999999</v>
+      </c>
+      <c r="H127" s="50">
+        <v>1404.2339999999999</v>
+      </c>
+      <c r="I127" s="50">
+        <v>1696.405</v>
+      </c>
+      <c r="J127" s="50">
+        <v>2020.893</v>
+      </c>
+      <c r="K127" s="50">
+        <v>2270.92</v>
+      </c>
+      <c r="L127" s="50">
+        <v>2392.2289999999998</v>
+      </c>
+      <c r="M127" s="50">
+        <v>2794.201</v>
+      </c>
+      <c r="N127" s="50">
+        <v>3132.962</v>
+      </c>
+      <c r="O127" s="50">
+        <v>3462.1089999999999</v>
+      </c>
+      <c r="P127" s="50">
+        <v>3544.5050000000001</v>
+      </c>
+      <c r="Q127" s="50">
+        <v>3558.3429999999998</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B128" s="46" t="s">
+        <v>463</v>
+      </c>
+      <c r="C128" s="50">
+        <v>354.14699999999999</v>
+      </c>
+      <c r="D128" s="50">
+        <v>478.06599999999997</v>
+      </c>
+      <c r="E128" s="50">
+        <v>620.524</v>
+      </c>
+      <c r="F128" s="50">
+        <v>745.995</v>
+      </c>
+      <c r="G128" s="50">
+        <v>897.00099999999998</v>
+      </c>
+      <c r="H128" s="50">
+        <v>1089.038</v>
+      </c>
+      <c r="I128" s="50">
+        <v>1350.6959999999999</v>
+      </c>
+      <c r="J128" s="50">
+        <v>1644.307</v>
+      </c>
+      <c r="K128" s="50">
+        <v>1960.962</v>
+      </c>
+      <c r="L128" s="50">
+        <v>2203.3530000000001</v>
+      </c>
+      <c r="M128" s="50">
+        <v>2309.2719999999999</v>
+      </c>
+      <c r="N128" s="50">
+        <v>2704.826</v>
+      </c>
+      <c r="O128" s="50">
+        <v>3062.1979999999999</v>
+      </c>
+      <c r="P128" s="50">
+        <v>3411.3249999999998</v>
+      </c>
+      <c r="Q128" s="50">
+        <v>3508.2669999999998</v>
+      </c>
+    </row>
+    <row r="129" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B129" s="46" t="s">
+        <v>341</v>
+      </c>
+      <c r="C129" s="50">
+        <v>326.98599999999999</v>
+      </c>
+      <c r="D129" s="50">
+        <v>341.363</v>
+      </c>
+      <c r="E129" s="50">
+        <v>463.54700000000003</v>
+      </c>
+      <c r="F129" s="50">
+        <v>604.98800000000006</v>
+      </c>
+      <c r="G129" s="50">
+        <v>730.43</v>
+      </c>
+      <c r="H129" s="50">
+        <v>881.66300000000001</v>
+      </c>
+      <c r="I129" s="50">
+        <v>1073.934</v>
+      </c>
+      <c r="J129" s="50">
+        <v>1335.3430000000001</v>
+      </c>
+      <c r="K129" s="50">
+        <v>1625.636</v>
+      </c>
+      <c r="L129" s="50">
+        <v>1937.1469999999999</v>
+      </c>
+      <c r="M129" s="50">
+        <v>2165.1869999999999</v>
+      </c>
+      <c r="N129" s="50">
+        <v>2267.56</v>
+      </c>
+      <c r="O129" s="50">
+        <v>2670.7550000000001</v>
+      </c>
+      <c r="P129" s="50">
+        <v>3040.2959999999998</v>
+      </c>
+      <c r="Q129" s="50">
+        <v>3395.31</v>
+      </c>
+    </row>
+    <row r="130" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B130" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="C130" s="50">
+        <v>316.221</v>
+      </c>
+      <c r="D130" s="50">
+        <v>318.005</v>
+      </c>
+      <c r="E130" s="50">
+        <v>333.24099999999999</v>
+      </c>
+      <c r="F130" s="50">
+        <v>453.52300000000002</v>
+      </c>
+      <c r="G130" s="50">
+        <v>593.84900000000005</v>
+      </c>
+      <c r="H130" s="50">
+        <v>719.10799999999995</v>
+      </c>
+      <c r="I130" s="50">
+        <v>870.702</v>
+      </c>
+      <c r="J130" s="50">
+        <v>1062.8620000000001</v>
+      </c>
+      <c r="K130" s="50">
+        <v>1321.492</v>
+      </c>
+      <c r="L130" s="50">
+        <v>1612.4110000000001</v>
+      </c>
+      <c r="M130" s="50">
+        <v>1905.8720000000001</v>
+      </c>
+      <c r="N130" s="50">
+        <v>2129.7710000000002</v>
+      </c>
+      <c r="O130" s="50">
+        <v>2234.4760000000001</v>
+      </c>
+      <c r="P130" s="50">
+        <v>2648.703</v>
+      </c>
+      <c r="Q130" s="50">
+        <v>3021.8609999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B131" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="C131" s="50">
+        <v>271.601</v>
+      </c>
+      <c r="D131" s="50">
+        <v>304.50299999999999</v>
+      </c>
+      <c r="E131" s="50">
+        <v>307.54399999999998</v>
+      </c>
+      <c r="F131" s="50">
+        <v>321.97500000000002</v>
+      </c>
+      <c r="G131" s="50">
+        <v>440.40600000000001</v>
+      </c>
+      <c r="H131" s="50">
+        <v>579.30499999999995</v>
+      </c>
+      <c r="I131" s="50">
+        <v>705.30899999999997</v>
+      </c>
+      <c r="J131" s="50">
+        <v>856.80399999999997</v>
+      </c>
+      <c r="K131" s="50">
+        <v>1045.797</v>
+      </c>
+      <c r="L131" s="50">
+        <v>1312.4690000000001</v>
+      </c>
+      <c r="M131" s="50">
+        <v>1572.5809999999999</v>
+      </c>
+      <c r="N131" s="50">
+        <v>1860.0509999999999</v>
+      </c>
+      <c r="O131" s="50">
+        <v>2074.1889999999999</v>
+      </c>
+      <c r="P131" s="50">
+        <v>2201.8820000000001</v>
+      </c>
+      <c r="Q131" s="50">
+        <v>2619.2020000000002</v>
+      </c>
+    </row>
+    <row r="132" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B132" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="C132" s="50">
+        <v>230.666</v>
+      </c>
+      <c r="D132" s="50">
+        <v>259.23099999999999</v>
+      </c>
+      <c r="E132" s="50">
+        <v>292.14100000000002</v>
+      </c>
+      <c r="F132" s="50">
+        <v>294.44799999999998</v>
+      </c>
+      <c r="G132" s="50">
+        <v>309.71800000000002</v>
+      </c>
+      <c r="H132" s="50">
+        <v>426.37599999999998</v>
+      </c>
+      <c r="I132" s="50">
+        <v>565.22</v>
+      </c>
+      <c r="J132" s="50">
+        <v>690.98599999999999</v>
+      </c>
+      <c r="K132" s="50">
+        <v>838.75599999999997</v>
+      </c>
+      <c r="L132" s="50">
+        <v>1037.9939999999999</v>
+      </c>
+      <c r="M132" s="50">
+        <v>1264.461</v>
+      </c>
+      <c r="N132" s="50">
+        <v>1517.6469999999999</v>
+      </c>
+      <c r="O132" s="50">
+        <v>1793.3610000000001</v>
+      </c>
+      <c r="P132" s="50">
+        <v>2032.4960000000001</v>
+      </c>
+      <c r="Q132" s="50">
+        <v>2167.181</v>
+      </c>
+    </row>
+    <row r="133" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B133" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="C133" s="50">
+        <v>199.917</v>
+      </c>
+      <c r="D133" s="50">
+        <v>219.32900000000001</v>
+      </c>
+      <c r="E133" s="50">
+        <v>247.82599999999999</v>
+      </c>
+      <c r="F133" s="50">
+        <v>278.96899999999999</v>
+      </c>
+      <c r="G133" s="50">
+        <v>282.46699999999998</v>
+      </c>
+      <c r="H133" s="50">
+        <v>298.673</v>
+      </c>
+      <c r="I133" s="50">
+        <v>414.83</v>
+      </c>
+      <c r="J133" s="50">
+        <v>552.23</v>
+      </c>
+      <c r="K133" s="50">
+        <v>673.80799999999999</v>
+      </c>
+      <c r="L133" s="50">
+        <v>827.22199999999998</v>
+      </c>
+      <c r="M133" s="50">
+        <v>986.48400000000004</v>
+      </c>
+      <c r="N133" s="50">
+        <v>1204.3820000000001</v>
+      </c>
+      <c r="O133" s="50">
+        <v>1454.2139999999999</v>
+      </c>
+      <c r="P133" s="50">
+        <v>1748.8420000000001</v>
+      </c>
+      <c r="Q133" s="50">
+        <v>1992.6479999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B134" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="C134" s="50">
+        <v>179.64400000000001</v>
+      </c>
+      <c r="D134" s="50">
+        <v>188.89400000000001</v>
+      </c>
+      <c r="E134" s="50">
+        <v>208.416</v>
+      </c>
+      <c r="F134" s="50">
+        <v>235.53399999999999</v>
+      </c>
+      <c r="G134" s="50">
+        <v>266.57400000000001</v>
+      </c>
+      <c r="H134" s="50">
+        <v>271.33800000000002</v>
+      </c>
+      <c r="I134" s="50">
+        <v>289.20600000000002</v>
+      </c>
+      <c r="J134" s="50">
+        <v>403.41500000000002</v>
+      </c>
+      <c r="K134" s="50">
+        <v>535.23599999999999</v>
+      </c>
+      <c r="L134" s="50">
+        <v>655.97500000000002</v>
+      </c>
+      <c r="M134" s="50">
+        <v>771.62599999999998</v>
+      </c>
+      <c r="N134" s="50">
+        <v>922.33500000000004</v>
+      </c>
+      <c r="O134" s="50">
+        <v>1145.7</v>
+      </c>
+      <c r="P134" s="50">
+        <v>1408.165</v>
+      </c>
+      <c r="Q134" s="50">
+        <v>1704.425</v>
+      </c>
+    </row>
+    <row r="135" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B135" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="C135" s="50">
+        <v>159.75800000000001</v>
+      </c>
+      <c r="D135" s="50">
+        <v>168.16800000000001</v>
+      </c>
+      <c r="E135" s="50">
+        <v>177.91399999999999</v>
+      </c>
+      <c r="F135" s="50">
+        <v>196.64699999999999</v>
+      </c>
+      <c r="G135" s="50">
+        <v>223.50899999999999</v>
+      </c>
+      <c r="H135" s="50">
+        <v>254.517</v>
+      </c>
+      <c r="I135" s="50">
+        <v>260.99</v>
+      </c>
+      <c r="J135" s="50">
+        <v>279.399</v>
+      </c>
+      <c r="K135" s="50">
+        <v>387.92099999999999</v>
+      </c>
+      <c r="L135" s="50">
+        <v>513.16899999999998</v>
+      </c>
+      <c r="M135" s="50">
+        <v>600</v>
+      </c>
+      <c r="N135" s="50">
+        <v>707.25699999999995</v>
+      </c>
+      <c r="O135" s="50">
+        <v>869.54499999999996</v>
+      </c>
+      <c r="P135" s="50">
+        <v>1099.9870000000001</v>
+      </c>
+      <c r="Q135" s="50">
+        <v>1362.4010000000001</v>
+      </c>
+    </row>
+    <row r="136" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B136" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="C136" s="50">
+        <v>132.405</v>
+      </c>
+      <c r="D136" s="50">
+        <v>147.99</v>
+      </c>
+      <c r="E136" s="50">
+        <v>156.77099999999999</v>
+      </c>
+      <c r="F136" s="50">
+        <v>166.37200000000001</v>
+      </c>
+      <c r="G136" s="50">
+        <v>184.96700000000001</v>
+      </c>
+      <c r="H136" s="50">
+        <v>211.59100000000001</v>
+      </c>
+      <c r="I136" s="50">
+        <v>242.727</v>
+      </c>
+      <c r="J136" s="50">
+        <v>250.02</v>
+      </c>
+      <c r="K136" s="50">
+        <v>266.21899999999999</v>
+      </c>
+      <c r="L136" s="50">
+        <v>367.01400000000001</v>
+      </c>
+      <c r="M136" s="50">
+        <v>462.19200000000001</v>
+      </c>
+      <c r="N136" s="50">
+        <v>541.072</v>
+      </c>
+      <c r="O136" s="50">
+        <v>660.13900000000001</v>
+      </c>
+      <c r="P136" s="50">
+        <v>826.80600000000004</v>
+      </c>
+      <c r="Q136" s="50">
+        <v>1055.1659999999999</v>
+      </c>
+    </row>
+    <row r="137" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B137" s="46" t="s">
+        <v>395</v>
+      </c>
+      <c r="C137" s="50">
+        <v>109.999</v>
+      </c>
+      <c r="D137" s="50">
+        <v>120.85</v>
+      </c>
+      <c r="E137" s="50">
+        <v>135.91200000000001</v>
+      </c>
+      <c r="F137" s="50">
+        <v>144.553</v>
+      </c>
+      <c r="G137" s="50">
+        <v>154.286</v>
+      </c>
+      <c r="H137" s="50">
+        <v>172.66499999999999</v>
+      </c>
+      <c r="I137" s="50">
+        <v>198.99600000000001</v>
+      </c>
+      <c r="J137" s="50">
+        <v>229.39599999999999</v>
+      </c>
+      <c r="K137" s="50">
+        <v>234.86</v>
+      </c>
+      <c r="L137" s="50">
+        <v>247.75700000000001</v>
+      </c>
+      <c r="M137" s="50">
+        <v>324.85899999999998</v>
+      </c>
+      <c r="N137" s="50">
+        <v>409.03199999999998</v>
+      </c>
+      <c r="O137" s="50">
+        <v>497.05700000000002</v>
+      </c>
+      <c r="P137" s="50">
+        <v>618.23699999999997</v>
+      </c>
+      <c r="Q137" s="50">
+        <v>782.09799999999996</v>
+      </c>
+    </row>
+    <row r="138" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B138" s="46" t="s">
+        <v>541</v>
+      </c>
+      <c r="C138" s="50">
+        <v>87.3</v>
+      </c>
+      <c r="D138" s="50">
+        <v>98.3</v>
+      </c>
+      <c r="E138" s="50">
+        <v>108.65300000000001</v>
+      </c>
+      <c r="F138" s="50">
+        <v>122.76900000000001</v>
+      </c>
+      <c r="G138" s="50">
+        <v>131.33600000000001</v>
+      </c>
+      <c r="H138" s="50">
+        <v>141.143</v>
+      </c>
+      <c r="I138" s="50">
+        <v>159.19300000000001</v>
+      </c>
+      <c r="J138" s="50">
+        <v>184.49199999999999</v>
+      </c>
+      <c r="K138" s="50">
+        <v>211.23500000000001</v>
+      </c>
+      <c r="L138" s="50">
+        <v>213.07400000000001</v>
+      </c>
+      <c r="M138" s="50">
+        <v>214.274</v>
+      </c>
+      <c r="N138" s="50">
+        <v>280.44099999999997</v>
+      </c>
+      <c r="O138" s="50">
+        <v>367.35899999999998</v>
+      </c>
+      <c r="P138" s="50">
+        <v>455.88299999999998</v>
+      </c>
+      <c r="Q138" s="50">
+        <v>573.69100000000003</v>
+      </c>
+    </row>
+    <row r="139" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B139" s="46" t="s">
+        <v>542</v>
+      </c>
+      <c r="C139" s="50">
+        <v>67.802000000000007</v>
+      </c>
+      <c r="D139" s="50">
+        <v>75.388000000000005</v>
+      </c>
+      <c r="E139" s="50">
+        <v>85.406999999999996</v>
+      </c>
+      <c r="F139" s="50">
+        <v>94.903999999999996</v>
+      </c>
+      <c r="G139" s="50">
+        <v>107.908</v>
+      </c>
+      <c r="H139" s="50">
+        <v>116.312</v>
+      </c>
+      <c r="I139" s="50">
+        <v>126.07899999999999</v>
+      </c>
+      <c r="J139" s="50">
+        <v>143.15600000000001</v>
+      </c>
+      <c r="K139" s="50">
+        <v>164.596</v>
+      </c>
+      <c r="L139" s="50">
+        <v>184.48099999999999</v>
+      </c>
+      <c r="M139" s="50">
+        <v>177.34200000000001</v>
+      </c>
+      <c r="N139" s="50">
+        <v>177.60400000000001</v>
+      </c>
+      <c r="O139" s="50">
+        <v>242.78299999999999</v>
+      </c>
+      <c r="P139" s="50">
+        <v>326.197</v>
+      </c>
+      <c r="Q139" s="50">
+        <v>410.863</v>
+      </c>
+    </row>
+    <row r="140" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B140" s="46" t="s">
+        <v>980</v>
+      </c>
+      <c r="C140" s="50">
+        <v>47.723999999999997</v>
+      </c>
+      <c r="D140" s="50">
+        <v>55.127000000000002</v>
+      </c>
+      <c r="E140" s="50">
+        <v>61.664000000000001</v>
+      </c>
+      <c r="F140" s="50">
+        <v>70.266000000000005</v>
+      </c>
+      <c r="G140" s="50">
+        <v>78.596999999999994</v>
+      </c>
+      <c r="H140" s="50">
+        <v>90.141000000000005</v>
+      </c>
+      <c r="I140" s="50">
+        <v>98.153999999999996</v>
+      </c>
+      <c r="J140" s="50">
+        <v>107.31399999999999</v>
+      </c>
+      <c r="K140" s="50">
+        <v>120.69799999999999</v>
+      </c>
+      <c r="L140" s="50">
+        <v>135.017</v>
+      </c>
+      <c r="M140" s="50">
+        <v>143.703</v>
+      </c>
+      <c r="N140" s="50">
+        <v>137.04300000000001</v>
+      </c>
+      <c r="O140" s="50">
+        <v>144.018</v>
+      </c>
+      <c r="P140" s="50">
+        <v>203.68700000000001</v>
+      </c>
+      <c r="Q140" s="50">
+        <v>279.48099999999999</v>
+      </c>
+    </row>
+    <row r="141" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B141" s="46" t="s">
+        <v>981</v>
+      </c>
+      <c r="C141" s="50">
+        <v>28.616</v>
+      </c>
+      <c r="D141" s="50">
+        <v>35.110999999999997</v>
+      </c>
+      <c r="E141" s="50">
+        <v>40.796999999999997</v>
+      </c>
+      <c r="F141" s="50">
+        <v>45.917000000000002</v>
+      </c>
+      <c r="G141" s="50">
+        <v>52.701000000000001</v>
+      </c>
+      <c r="H141" s="50">
+        <v>59.548999999999999</v>
+      </c>
+      <c r="I141" s="50">
+        <v>69.17</v>
+      </c>
+      <c r="J141" s="50">
+        <v>76.191000000000003</v>
+      </c>
+      <c r="K141" s="50">
+        <v>82.307000000000002</v>
+      </c>
+      <c r="L141" s="50">
+        <v>89.284999999999997</v>
+      </c>
+      <c r="M141" s="50">
+        <v>94.103999999999999</v>
+      </c>
+      <c r="N141" s="50">
+        <v>98.856999999999999</v>
+      </c>
+      <c r="O141" s="50">
+        <v>99.944000000000003</v>
+      </c>
+      <c r="P141" s="50">
+        <v>110.20399999999999</v>
+      </c>
+      <c r="Q141" s="50">
+        <v>161.035</v>
+      </c>
+    </row>
+    <row r="142" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B142" s="46" t="s">
+        <v>982</v>
+      </c>
+      <c r="C142" s="50">
+        <v>14.840999999999999</v>
+      </c>
+      <c r="D142" s="50">
+        <v>17.861999999999998</v>
+      </c>
+      <c r="E142" s="50">
+        <v>22.023</v>
+      </c>
+      <c r="F142" s="50">
+        <v>25.728000000000002</v>
+      </c>
+      <c r="G142" s="50">
+        <v>29.167000000000002</v>
+      </c>
+      <c r="H142" s="50">
+        <v>33.866</v>
+      </c>
+      <c r="I142" s="50">
+        <v>38.892000000000003</v>
+      </c>
+      <c r="J142" s="50">
+        <v>45.896000000000001</v>
+      </c>
+      <c r="K142" s="50">
+        <v>49.774999999999999</v>
+      </c>
+      <c r="L142" s="50">
+        <v>51.314</v>
+      </c>
+      <c r="M142" s="50">
+        <v>51.887999999999998</v>
+      </c>
+      <c r="N142" s="50">
+        <v>53.573</v>
+      </c>
+      <c r="O142" s="50">
+        <v>60.344999999999999</v>
+      </c>
+      <c r="P142" s="50">
+        <v>65.712999999999994</v>
+      </c>
+      <c r="Q142" s="50">
+        <v>76.403999999999996</v>
+      </c>
+    </row>
+    <row r="143" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B143" s="46" t="s">
+        <v>331</v>
+      </c>
+      <c r="C143" s="37">
+        <v>6.7920000000000007</v>
+      </c>
+      <c r="D143" s="37">
+        <v>8.9410000000000007</v>
+      </c>
+      <c r="E143" s="37">
+        <v>11.025</v>
+      </c>
+      <c r="F143" s="37">
+        <v>13.533999999999997</v>
+      </c>
+      <c r="G143" s="37">
+        <v>16.044999999999998</v>
+      </c>
+      <c r="H143" s="37">
+        <v>18.555000000000003</v>
+      </c>
+      <c r="I143" s="37">
+        <v>21.943000000000001</v>
+      </c>
+      <c r="J143" s="37">
+        <v>25.936</v>
+      </c>
+      <c r="K143" s="37">
+        <v>29.832999999999998</v>
+      </c>
+      <c r="L143" s="37">
+        <v>30.677999999999997</v>
+      </c>
+      <c r="M143" s="37">
+        <v>28.76</v>
+      </c>
+      <c r="N143" s="37">
+        <v>27.613</v>
+      </c>
+      <c r="O143" s="37">
+        <v>30.65</v>
+      </c>
+      <c r="P143" s="37">
+        <v>39.680999999999997</v>
+      </c>
+      <c r="Q143" s="37">
+        <v>50.151000000000003</v>
+      </c>
+    </row>
+    <row r="144" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B144" s="50"/>
+      <c r="C144" s="50"/>
+      <c r="D144" s="50"/>
+      <c r="E144" s="50"/>
+      <c r="F144" s="50"/>
+      <c r="G144" s="50"/>
+      <c r="H144" s="50"/>
+      <c r="I144" s="50"/>
+      <c r="J144" s="50"/>
+      <c r="K144" s="50"/>
+      <c r="L144" s="50"/>
+      <c r="M144" s="50"/>
+      <c r="N144" s="50"/>
+      <c r="O144" s="50"/>
+      <c r="P144" s="50"/>
+    </row>
+    <row r="145" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B145" s="37" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C145" s="47">
+        <v>1950</v>
+      </c>
+      <c r="D145" s="47">
+        <v>1955</v>
+      </c>
+      <c r="E145" s="47">
+        <v>1960</v>
+      </c>
+      <c r="F145" s="47">
+        <v>1965</v>
+      </c>
+      <c r="G145" s="47">
+        <v>1970</v>
+      </c>
+      <c r="H145" s="47">
+        <v>1975</v>
+      </c>
+      <c r="I145" s="47">
+        <v>1980</v>
+      </c>
+      <c r="J145" s="47">
+        <v>1985</v>
+      </c>
+      <c r="K145" s="47">
+        <v>1990</v>
+      </c>
+      <c r="L145" s="47">
+        <v>1995</v>
+      </c>
+      <c r="M145" s="47">
+        <v>2000</v>
+      </c>
+      <c r="N145" s="47">
+        <v>2005</v>
+      </c>
+      <c r="O145" s="47">
+        <v>2010</v>
+      </c>
+      <c r="P145" s="47">
+        <v>2015</v>
+      </c>
+      <c r="Q145" s="47">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="146" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B146" s="46" t="s">
+        <v>499</v>
+      </c>
+      <c r="C146" s="50">
+        <v>526.12800000000004</v>
+      </c>
+      <c r="D146" s="50">
+        <v>678.548</v>
+      </c>
+      <c r="E146" s="50">
+        <v>800.50300000000004</v>
+      </c>
+      <c r="F146" s="50">
+        <v>951.90099999999995</v>
+      </c>
+      <c r="G146" s="50">
+        <v>1138.8889999999999</v>
+      </c>
+      <c r="H146" s="50">
+        <v>1394.3009999999999</v>
+      </c>
+      <c r="I146" s="50">
+        <v>1677.8230000000001</v>
+      </c>
+      <c r="J146" s="50">
+        <v>1992.7149999999999</v>
+      </c>
+      <c r="K146" s="50">
+        <v>2237.337</v>
+      </c>
+      <c r="L146" s="50">
+        <v>2353.848</v>
+      </c>
+      <c r="M146" s="50">
+        <v>2744.68</v>
+      </c>
+      <c r="N146" s="50">
+        <v>3075.279</v>
+      </c>
+      <c r="O146" s="50">
+        <v>3390.8629999999998</v>
+      </c>
+      <c r="P146" s="50">
+        <v>3491.221</v>
+      </c>
+      <c r="Q146" s="50">
+        <v>3486.0210000000002</v>
+      </c>
+    </row>
+    <row r="147" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B147" s="46" t="s">
+        <v>463</v>
+      </c>
+      <c r="C147" s="50">
+        <v>352.59500000000003</v>
+      </c>
+      <c r="D147" s="50">
+        <v>478.45</v>
+      </c>
+      <c r="E147" s="50">
+        <v>625.42399999999998</v>
+      </c>
+      <c r="F147" s="50">
+        <v>750.63900000000001</v>
+      </c>
+      <c r="G147" s="50">
+        <v>902.67200000000003</v>
+      </c>
+      <c r="H147" s="50">
+        <v>1091.424</v>
+      </c>
+      <c r="I147" s="50">
+        <v>1346.829</v>
+      </c>
+      <c r="J147" s="50">
+        <v>1631.4639999999999</v>
+      </c>
+      <c r="K147" s="50">
+        <v>1940.953</v>
+      </c>
+      <c r="L147" s="50">
+        <v>2183.0940000000001</v>
+      </c>
+      <c r="M147" s="50">
+        <v>2290.3620000000001</v>
+      </c>
+      <c r="N147" s="50">
+        <v>2678.6390000000001</v>
+      </c>
+      <c r="O147" s="50">
+        <v>3018.3670000000002</v>
+      </c>
+      <c r="P147" s="50">
+        <v>3353.1439999999998</v>
+      </c>
+      <c r="Q147" s="50">
+        <v>3461.279</v>
+      </c>
+    </row>
+    <row r="148" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B148" s="46" t="s">
+        <v>341</v>
+      </c>
+      <c r="C148" s="50">
+        <v>326.79300000000001</v>
+      </c>
+      <c r="D148" s="50">
+        <v>339.952</v>
+      </c>
+      <c r="E148" s="50">
+        <v>464.02</v>
+      </c>
+      <c r="F148" s="50">
+        <v>610.71199999999999</v>
+      </c>
+      <c r="G148" s="50">
+        <v>736.11599999999999</v>
+      </c>
+      <c r="H148" s="50">
+        <v>888.49599999999998</v>
+      </c>
+      <c r="I148" s="50">
+        <v>1077.318</v>
+      </c>
+      <c r="J148" s="50">
+        <v>1332.5719999999999</v>
+      </c>
+      <c r="K148" s="50">
+        <v>1615.5360000000001</v>
+      </c>
+      <c r="L148" s="50">
+        <v>1924.5530000000001</v>
+      </c>
+      <c r="M148" s="50">
+        <v>2159.6559999999999</v>
+      </c>
+      <c r="N148" s="50">
+        <v>2265.5639999999999</v>
+      </c>
+      <c r="O148" s="50">
+        <v>2654.402</v>
+      </c>
+      <c r="P148" s="50">
+        <v>3001.846</v>
+      </c>
+      <c r="Q148" s="50">
+        <v>3340.913</v>
+      </c>
+    </row>
+    <row r="149" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B149" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="C149" s="50">
+        <v>306.90800000000002</v>
+      </c>
+      <c r="D149" s="50">
+        <v>317.78699999999998</v>
+      </c>
+      <c r="E149" s="50">
+        <v>331.92099999999999</v>
+      </c>
+      <c r="F149" s="50">
+        <v>454.77800000000002</v>
+      </c>
+      <c r="G149" s="50">
+        <v>600.572</v>
+      </c>
+      <c r="H149" s="50">
+        <v>726.02300000000002</v>
+      </c>
+      <c r="I149" s="50">
+        <v>878.62300000000005</v>
+      </c>
+      <c r="J149" s="50">
+        <v>1067.5150000000001</v>
+      </c>
+      <c r="K149" s="50">
+        <v>1321.2439999999999</v>
+      </c>
+      <c r="L149" s="50">
+        <v>1608.7</v>
+      </c>
+      <c r="M149" s="50">
+        <v>1904.5170000000001</v>
+      </c>
+      <c r="N149" s="50">
+        <v>2137.7130000000002</v>
+      </c>
+      <c r="O149" s="50">
+        <v>2242.0169999999998</v>
+      </c>
+      <c r="P149" s="50">
+        <v>2638.4279999999999</v>
+      </c>
+      <c r="Q149" s="50">
+        <v>2988.7950000000001</v>
+      </c>
+    </row>
+    <row r="150" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B150" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="C150" s="50">
+        <v>254.81899999999999</v>
+      </c>
+      <c r="D150" s="50">
+        <v>297.32299999999998</v>
+      </c>
+      <c r="E150" s="50">
+        <v>309.05700000000002</v>
+      </c>
+      <c r="F150" s="50">
+        <v>323.12</v>
+      </c>
+      <c r="G150" s="50">
+        <v>444.61799999999999</v>
+      </c>
+      <c r="H150" s="50">
+        <v>589.40099999999995</v>
+      </c>
+      <c r="I150" s="50">
+        <v>715.35199999999998</v>
+      </c>
+      <c r="J150" s="50">
+        <v>868.02700000000004</v>
+      </c>
+      <c r="K150" s="50">
+        <v>1055.079</v>
+      </c>
+      <c r="L150" s="50">
+        <v>1320.759</v>
+      </c>
+      <c r="M150" s="50">
+        <v>1580.1079999999999</v>
+      </c>
+      <c r="N150" s="50">
+        <v>1872.1189999999999</v>
+      </c>
+      <c r="O150" s="50">
+        <v>2097.8389999999999</v>
+      </c>
+      <c r="P150" s="50">
+        <v>2218.2339999999999</v>
+      </c>
+      <c r="Q150" s="50">
+        <v>2617.3910000000001</v>
+      </c>
+    </row>
+    <row r="151" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B151" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="C151" s="50">
+        <v>207.57900000000001</v>
+      </c>
+      <c r="D151" s="50">
+        <v>245.5</v>
+      </c>
+      <c r="E151" s="50">
+        <v>287.62099999999998</v>
+      </c>
+      <c r="F151" s="50">
+        <v>298.97699999999998</v>
+      </c>
+      <c r="G151" s="50">
+        <v>313.76499999999999</v>
+      </c>
+      <c r="H151" s="50">
+        <v>433.89800000000002</v>
+      </c>
+      <c r="I151" s="50">
+        <v>578.34500000000003</v>
+      </c>
+      <c r="J151" s="50">
+        <v>704.22799999999995</v>
+      </c>
+      <c r="K151" s="50">
+        <v>854.32600000000002</v>
+      </c>
+      <c r="L151" s="50">
+        <v>1054.078</v>
+      </c>
+      <c r="M151" s="50">
+        <v>1278.6389999999999</v>
+      </c>
+      <c r="N151" s="50">
+        <v>1529.6469999999999</v>
+      </c>
+      <c r="O151" s="50">
+        <v>1818.0820000000001</v>
+      </c>
+      <c r="P151" s="50">
+        <v>2063.39</v>
+      </c>
+      <c r="Q151" s="50">
+        <v>2190.5</v>
+      </c>
+    </row>
+    <row r="152" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B152" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="C152" s="50">
+        <v>178.965</v>
+      </c>
+      <c r="D152" s="50">
+        <v>198.82499999999999</v>
+      </c>
+      <c r="E152" s="50">
+        <v>236.2</v>
+      </c>
+      <c r="F152" s="50">
+        <v>277.012</v>
+      </c>
+      <c r="G152" s="50">
+        <v>289.12599999999998</v>
+      </c>
+      <c r="H152" s="50">
+        <v>304.75599999999997</v>
+      </c>
+      <c r="I152" s="50">
+        <v>424.13600000000002</v>
+      </c>
+      <c r="J152" s="50">
+        <v>567.375</v>
+      </c>
+      <c r="K152" s="50">
+        <v>690.19899999999996</v>
+      </c>
+      <c r="L152" s="50">
+        <v>847.08799999999997</v>
+      </c>
+      <c r="M152" s="50">
+        <v>1003.39</v>
+      </c>
+      <c r="N152" s="50">
+        <v>1214.3209999999999</v>
+      </c>
+      <c r="O152" s="50">
+        <v>1472.3409999999999</v>
+      </c>
+      <c r="P152" s="50">
+        <v>1778.5409999999999</v>
+      </c>
+      <c r="Q152" s="50">
+        <v>2030.0440000000001</v>
+      </c>
+    </row>
+    <row r="153" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B153" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="C153" s="50">
+        <v>155.19999999999999</v>
+      </c>
+      <c r="D153" s="50">
+        <v>170.417</v>
+      </c>
+      <c r="E153" s="50">
+        <v>190.23400000000001</v>
+      </c>
+      <c r="F153" s="50">
+        <v>226.46600000000001</v>
+      </c>
+      <c r="G153" s="50">
+        <v>266.87</v>
+      </c>
+      <c r="H153" s="50">
+        <v>279.83499999999998</v>
+      </c>
+      <c r="I153" s="50">
+        <v>296.69</v>
+      </c>
+      <c r="J153" s="50">
+        <v>414.51299999999998</v>
+      </c>
+      <c r="K153" s="50">
+        <v>553.59100000000001</v>
+      </c>
+      <c r="L153" s="50">
+        <v>677.15700000000004</v>
+      </c>
+      <c r="M153" s="50">
+        <v>793.59900000000005</v>
+      </c>
+      <c r="N153" s="50">
+        <v>935.38099999999997</v>
+      </c>
+      <c r="O153" s="50">
+        <v>1159.8579999999999</v>
+      </c>
+      <c r="P153" s="50">
+        <v>1432.489</v>
+      </c>
+      <c r="Q153" s="50">
+        <v>1743.029</v>
+      </c>
+    </row>
+    <row r="154" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B154" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="C154" s="50">
+        <v>140.553</v>
+      </c>
+      <c r="D154" s="50">
+        <v>146.87799999999999</v>
+      </c>
+      <c r="E154" s="50">
+        <v>162.05699999999999</v>
+      </c>
+      <c r="F154" s="50">
+        <v>181.434</v>
+      </c>
+      <c r="G154" s="50">
+        <v>217.05099999999999</v>
+      </c>
+      <c r="H154" s="50">
+        <v>257.08800000000002</v>
+      </c>
+      <c r="I154" s="50">
+        <v>271.05</v>
+      </c>
+      <c r="J154" s="50">
+        <v>288.54000000000002</v>
+      </c>
+      <c r="K154" s="50">
+        <v>402.33699999999999</v>
+      </c>
+      <c r="L154" s="50">
+        <v>537.63199999999995</v>
+      </c>
+      <c r="M154" s="50">
+        <v>628.12400000000002</v>
+      </c>
+      <c r="N154" s="50">
+        <v>731.42600000000004</v>
+      </c>
+      <c r="O154" s="50">
+        <v>887.47500000000002</v>
+      </c>
+      <c r="P154" s="50">
+        <v>1121.7439999999999</v>
+      </c>
+      <c r="Q154" s="50">
+        <v>1397.049</v>
+      </c>
+    </row>
+    <row r="155" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B155" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="C155" s="50">
+        <v>130.56100000000001</v>
+      </c>
+      <c r="D155" s="50">
+        <v>132.35300000000001</v>
+      </c>
+      <c r="E155" s="50">
+        <v>138.94300000000001</v>
+      </c>
+      <c r="F155" s="50">
+        <v>153.845</v>
+      </c>
+      <c r="G155" s="50">
+        <v>173.035</v>
+      </c>
+      <c r="H155" s="50">
+        <v>208.06200000000001</v>
+      </c>
+      <c r="I155" s="50">
+        <v>247.74600000000001</v>
+      </c>
+      <c r="J155" s="50">
+        <v>262.26400000000001</v>
+      </c>
+      <c r="K155" s="50">
+        <v>278.68299999999999</v>
+      </c>
+      <c r="L155" s="50">
+        <v>388.214</v>
+      </c>
+      <c r="M155" s="50">
+        <v>497.30700000000002</v>
+      </c>
+      <c r="N155" s="50">
+        <v>577.23500000000001</v>
+      </c>
+      <c r="O155" s="50">
+        <v>690.89400000000001</v>
+      </c>
+      <c r="P155" s="50">
+        <v>853.59100000000001</v>
+      </c>
+      <c r="Q155" s="50">
+        <v>1088.4290000000001</v>
+      </c>
+    </row>
+    <row r="156" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B156" s="46" t="s">
+        <v>395</v>
+      </c>
+      <c r="C156" s="50">
+        <v>116.206</v>
+      </c>
+      <c r="D156" s="50">
+        <v>121.746</v>
+      </c>
+      <c r="E156" s="50">
+        <v>123.979</v>
+      </c>
+      <c r="F156" s="50">
+        <v>130.71299999999999</v>
+      </c>
+      <c r="G156" s="50">
+        <v>145.41</v>
+      </c>
+      <c r="H156" s="50">
+        <v>164.40799999999999</v>
+      </c>
+      <c r="I156" s="50">
+        <v>198.756</v>
+      </c>
+      <c r="J156" s="50">
+        <v>237.71</v>
+      </c>
+      <c r="K156" s="50">
+        <v>251.215</v>
+      </c>
+      <c r="L156" s="50">
+        <v>266.464</v>
+      </c>
+      <c r="M156" s="50">
+        <v>356.84699999999998</v>
+      </c>
+      <c r="N156" s="50">
+        <v>454.13400000000001</v>
+      </c>
+      <c r="O156" s="50">
+        <v>541.01400000000001</v>
+      </c>
+      <c r="P156" s="50">
+        <v>658.98800000000006</v>
+      </c>
+      <c r="Q156" s="50">
+        <v>821.97500000000002</v>
+      </c>
+    </row>
+    <row r="157" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B157" s="46" t="s">
+        <v>541</v>
+      </c>
+      <c r="C157" s="50">
+        <v>97</v>
+      </c>
+      <c r="D157" s="50">
+        <v>106.303</v>
+      </c>
+      <c r="E157" s="50">
+        <v>111.93899999999999</v>
+      </c>
+      <c r="F157" s="50">
+        <v>114.639</v>
+      </c>
+      <c r="G157" s="50">
+        <v>121.511</v>
+      </c>
+      <c r="H157" s="50">
+        <v>135.994</v>
+      </c>
+      <c r="I157" s="50">
+        <v>154.68299999999999</v>
+      </c>
+      <c r="J157" s="50">
+        <v>188.00700000000001</v>
+      </c>
+      <c r="K157" s="50">
+        <v>224.55600000000001</v>
+      </c>
+      <c r="L157" s="50">
+        <v>236.12899999999999</v>
+      </c>
+      <c r="M157" s="50">
+        <v>242.233</v>
+      </c>
+      <c r="N157" s="50">
+        <v>322.36399999999998</v>
+      </c>
+      <c r="O157" s="50">
+        <v>420.16199999999998</v>
+      </c>
+      <c r="P157" s="50">
+        <v>509.68400000000003</v>
+      </c>
+      <c r="Q157" s="50">
+        <v>627.83900000000006</v>
+      </c>
+    </row>
+    <row r="158" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B158" s="46" t="s">
+        <v>542</v>
+      </c>
+      <c r="C158" s="50">
+        <v>78.376000000000005</v>
+      </c>
+      <c r="D158" s="50">
+        <v>85.778999999999996</v>
+      </c>
+      <c r="E158" s="50">
+        <v>94.581999999999994</v>
+      </c>
+      <c r="F158" s="50">
+        <v>100.371</v>
+      </c>
+      <c r="G158" s="50">
+        <v>103.48099999999999</v>
+      </c>
+      <c r="H158" s="50">
+        <v>110.515</v>
+      </c>
+      <c r="I158" s="50">
+        <v>124.60299999999999</v>
+      </c>
+      <c r="J158" s="50">
+        <v>142.73599999999999</v>
+      </c>
+      <c r="K158" s="50">
+        <v>173.36699999999999</v>
+      </c>
+      <c r="L158" s="50">
+        <v>205.55199999999999</v>
+      </c>
+      <c r="M158" s="50">
+        <v>209.96299999999999</v>
+      </c>
+      <c r="N158" s="50">
+        <v>214.01499999999999</v>
+      </c>
+      <c r="O158" s="50">
+        <v>291.30700000000002</v>
+      </c>
+      <c r="P158" s="50">
+        <v>387.77100000000002</v>
+      </c>
+      <c r="Q158" s="50">
+        <v>477.35199999999998</v>
+      </c>
+    </row>
+    <row r="159" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B159" s="46" t="s">
+        <v>980</v>
+      </c>
+      <c r="C159" s="50">
+        <v>60.14</v>
+      </c>
+      <c r="D159" s="50">
+        <v>65.23</v>
+      </c>
+      <c r="E159" s="50">
+        <v>71.912000000000006</v>
+      </c>
+      <c r="F159" s="50">
+        <v>80.097999999999999</v>
+      </c>
+      <c r="G159" s="50">
+        <v>85.733000000000004</v>
+      </c>
+      <c r="H159" s="50">
+        <v>89.266999999999996</v>
+      </c>
+      <c r="I159" s="50">
+        <v>96.26</v>
+      </c>
+      <c r="J159" s="50">
+        <v>109.626</v>
+      </c>
+      <c r="K159" s="50">
+        <v>125.645</v>
+      </c>
+      <c r="L159" s="50">
+        <v>151.38499999999999</v>
+      </c>
+      <c r="M159" s="50">
+        <v>174.976</v>
+      </c>
+      <c r="N159" s="50">
+        <v>177.5</v>
+      </c>
+      <c r="O159" s="50">
+        <v>184.685</v>
+      </c>
+      <c r="P159" s="50">
+        <v>258.214</v>
+      </c>
+      <c r="Q159" s="50">
+        <v>351.13</v>
+      </c>
+    </row>
+    <row r="160" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B160" s="46" t="s">
+        <v>981</v>
+      </c>
+      <c r="C160" s="50">
+        <v>40.061</v>
+      </c>
+      <c r="D160" s="50">
+        <v>45.283999999999999</v>
+      </c>
+      <c r="E160" s="50">
+        <v>49.512</v>
+      </c>
+      <c r="F160" s="50">
+        <v>55.249000000000002</v>
+      </c>
+      <c r="G160" s="50">
+        <v>62.197000000000003</v>
+      </c>
+      <c r="H160" s="50">
+        <v>67.433999999999997</v>
+      </c>
+      <c r="I160" s="50">
+        <v>71.120999999999995</v>
+      </c>
+      <c r="J160" s="50">
+        <v>77.8</v>
+      </c>
+      <c r="K160" s="50">
+        <v>88.807000000000002</v>
+      </c>
+      <c r="L160" s="50">
+        <v>100.953</v>
+      </c>
+      <c r="M160" s="50">
+        <v>119.01600000000001</v>
+      </c>
+      <c r="N160" s="50">
+        <v>136.50700000000001</v>
+      </c>
+      <c r="O160" s="50">
+        <v>141.065</v>
+      </c>
+      <c r="P160" s="50">
+        <v>152.22</v>
+      </c>
+      <c r="Q160" s="50">
+        <v>220.03200000000001</v>
+      </c>
+    </row>
+    <row r="161" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B161" s="46" t="s">
+        <v>982</v>
+      </c>
+      <c r="C161" s="50">
+        <v>26.19</v>
+      </c>
+      <c r="D161" s="50">
+        <v>25.728000000000002</v>
+      </c>
+      <c r="E161" s="50">
+        <v>29.297999999999998</v>
+      </c>
+      <c r="F161" s="50">
+        <v>32.44</v>
+      </c>
+      <c r="G161" s="50">
+        <v>36.642000000000003</v>
+      </c>
+      <c r="H161" s="50">
+        <v>41.908999999999999</v>
+      </c>
+      <c r="I161" s="50">
+        <v>46.204999999999998</v>
+      </c>
+      <c r="J161" s="50">
+        <v>49.720999999999997</v>
+      </c>
+      <c r="K161" s="50">
+        <v>54.652999999999999</v>
+      </c>
+      <c r="L161" s="50">
+        <v>61.912999999999997</v>
+      </c>
+      <c r="M161" s="50">
+        <v>69.313999999999993</v>
+      </c>
+      <c r="N161" s="50">
+        <v>81.033000000000001</v>
+      </c>
+      <c r="O161" s="50">
+        <v>94.150999999999996</v>
+      </c>
+      <c r="P161" s="50">
+        <v>102.624</v>
+      </c>
+      <c r="Q161" s="50">
+        <v>116.86799999999999</v>
+      </c>
+    </row>
+    <row r="162" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B162" s="46" t="s">
+        <v>331</v>
+      </c>
+      <c r="C162" s="50">
+        <v>14.159999999999998</v>
+      </c>
+      <c r="D162" s="50">
+        <v>16.881</v>
+      </c>
+      <c r="E162" s="50">
+        <v>17.580000000000005</v>
+      </c>
+      <c r="F162" s="50">
+        <v>19.491</v>
+      </c>
+      <c r="G162" s="50">
+        <v>21.837</v>
+      </c>
+      <c r="H162" s="50">
+        <v>25.012999999999998</v>
+      </c>
+      <c r="I162" s="50">
+        <v>29.216999999999999</v>
+      </c>
+      <c r="J162" s="50">
+        <v>33.625</v>
+      </c>
+      <c r="K162" s="50">
+        <v>36.995000000000005</v>
+      </c>
+      <c r="L162" s="50">
+        <v>40.189</v>
+      </c>
+      <c r="M162" s="50">
+        <v>45.019999999999989</v>
+      </c>
+      <c r="N162" s="50">
+        <v>49.994</v>
+      </c>
+      <c r="O162" s="50">
+        <v>57.32</v>
+      </c>
+      <c r="P162" s="50">
+        <v>73.600999999999999</v>
+      </c>
+      <c r="Q162" s="50">
+        <v>94.126999999999995</v>
+      </c>
+    </row>
+    <row r="163" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B163" s="50"/>
+      <c r="C163" s="50"/>
+      <c r="D163" s="50"/>
+      <c r="E163" s="50"/>
+      <c r="F163" s="50"/>
+      <c r="G163" s="50"/>
+      <c r="H163" s="50"/>
+      <c r="I163" s="50"/>
+      <c r="J163" s="50"/>
+      <c r="K163" s="50"/>
+      <c r="L163" s="50"/>
+      <c r="M163" s="50"/>
+      <c r="N163" s="50"/>
+      <c r="O163" s="50"/>
+      <c r="P163" s="50"/>
+    </row>
+    <row r="164" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B164" s="50"/>
+      <c r="C164" s="50"/>
+      <c r="D164" s="50"/>
+      <c r="E164" s="50"/>
+      <c r="F164" s="50"/>
+      <c r="G164" s="50"/>
+      <c r="H164" s="50"/>
+      <c r="I164" s="50"/>
+      <c r="J164" s="50"/>
+      <c r="K164" s="50"/>
+      <c r="L164" s="50"/>
+      <c r="M164" s="50"/>
+      <c r="N164" s="50"/>
+      <c r="O164" s="50"/>
+      <c r="P164" s="50"/>
+    </row>
+    <row r="165" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B165" s="50"/>
+      <c r="C165" s="50"/>
+      <c r="D165" s="50"/>
+      <c r="E165" s="50"/>
+      <c r="F165" s="50"/>
+      <c r="G165" s="50"/>
+      <c r="H165" s="50"/>
+      <c r="I165" s="50"/>
+      <c r="J165" s="50"/>
+      <c r="K165" s="50"/>
+      <c r="L165" s="50"/>
+      <c r="M165" s="50"/>
+      <c r="N165" s="50"/>
+      <c r="O165" s="50"/>
+      <c r="P165" s="50"/>
+    </row>
+    <row r="166" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B166" s="50"/>
+      <c r="C166" s="50"/>
+      <c r="D166" s="50"/>
+      <c r="E166" s="50"/>
+      <c r="F166" s="50"/>
+      <c r="G166" s="50"/>
+      <c r="H166" s="50"/>
+      <c r="I166" s="50"/>
+      <c r="J166" s="50"/>
+      <c r="K166" s="50"/>
+      <c r="L166" s="50"/>
+      <c r="M166" s="50"/>
+      <c r="N166" s="50"/>
+      <c r="O166" s="50"/>
+      <c r="P166" s="50"/>
+    </row>
+    <row r="168" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C168" s="51"/>
+      <c r="D168" s="51"/>
+      <c r="E168" s="51"/>
+      <c r="F168" s="51"/>
+      <c r="G168" s="51"/>
+      <c r="H168" s="51"/>
+      <c r="I168" s="51"/>
+      <c r="J168" s="51"/>
+      <c r="K168" s="51"/>
+      <c r="L168" s="51"/>
+      <c r="M168" s="51"/>
+      <c r="N168" s="51"/>
+      <c r="O168" s="51"/>
+      <c r="P168" s="51"/>
+      <c r="Q168" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28385,11 +30319,11 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C18" s="45">
+      <c r="C18" s="49">
         <v>2015</v>
       </c>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
       <c r="G18" s="23">
         <v>2013</v>
       </c>
@@ -36019,10 +37953,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG100"/>
+  <dimension ref="A1:AG119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="J129" sqref="J129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36971,6 +38905,7 @@
         <f t="shared" si="10"/>
         <v>7.3389999999999997E-2</v>
       </c>
+      <c r="J45" s="48"/>
       <c r="Q45" s="22" t="s">
         <v>137</v>
       </c>
@@ -37055,6 +38990,7 @@
         <f t="shared" si="10"/>
         <v>0.15087999999999999</v>
       </c>
+      <c r="J46" s="48"/>
       <c r="Q46" s="21" t="s">
         <v>138</v>
       </c>
@@ -37139,6 +39075,7 @@
         <f t="shared" si="10"/>
         <v>0.15251999999999999</v>
       </c>
+      <c r="J47" s="48"/>
       <c r="Q47" s="21" t="s">
         <v>139</v>
       </c>
@@ -37223,6 +39160,7 @@
         <f t="shared" si="10"/>
         <v>0.12750999999999998</v>
       </c>
+      <c r="J48" s="48"/>
       <c r="Q48" s="21" t="s">
         <v>140</v>
       </c>
@@ -37307,6 +39245,7 @@
         <f t="shared" si="10"/>
         <v>9.2659999999999992E-2</v>
       </c>
+      <c r="J49" s="48"/>
       <c r="Q49" s="21" t="s">
         <v>141</v>
       </c>
@@ -37391,6 +39330,7 @@
         <f t="shared" si="10"/>
         <v>4.3049999999999998E-2</v>
       </c>
+      <c r="J50" s="48"/>
       <c r="Q50" s="21" t="s">
         <v>142</v>
       </c>
@@ -37475,6 +39415,7 @@
         <f t="shared" si="10"/>
         <v>5.7399999999999994E-3</v>
       </c>
+      <c r="J51" s="48"/>
       <c r="K51" t="s">
         <v>456</v>
       </c>
@@ -38337,763 +40278,1305 @@
       </c>
     </row>
     <row r="93" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B93" s="46" t="s">
+      <c r="B93" s="45" t="s">
         <v>1050</v>
       </c>
-      <c r="C93" s="48" t="s">
+      <c r="C93" s="47" t="s">
         <v>1051</v>
       </c>
-      <c r="D93" s="48" t="s">
+      <c r="D93" s="47" t="s">
         <v>1052</v>
       </c>
-      <c r="E93" s="48" t="s">
+      <c r="E93" s="47" t="s">
         <v>1053</v>
       </c>
-      <c r="F93" s="48" t="s">
+      <c r="F93" s="47" t="s">
         <v>1054</v>
       </c>
-      <c r="G93" s="48" t="s">
+      <c r="G93" s="47" t="s">
         <v>1055</v>
       </c>
-      <c r="H93" s="48" t="s">
+      <c r="H93" s="47" t="s">
         <v>1056</v>
       </c>
-      <c r="I93" s="48" t="s">
+      <c r="I93" s="47" t="s">
         <v>1057</v>
       </c>
-      <c r="J93" s="48" t="s">
+      <c r="J93" s="47" t="s">
         <v>1058</v>
       </c>
-      <c r="K93" s="48" t="s">
+      <c r="K93" s="47" t="s">
         <v>1059</v>
       </c>
-      <c r="L93" s="48" t="s">
+      <c r="L93" s="47" t="s">
         <v>1060</v>
       </c>
-      <c r="M93" s="48" t="s">
+      <c r="M93" s="47" t="s">
         <v>1061</v>
       </c>
-      <c r="N93" s="48" t="s">
+      <c r="N93" s="47" t="s">
         <v>1062</v>
       </c>
-      <c r="O93" s="48" t="s">
+      <c r="O93" s="47" t="s">
         <v>1063</v>
       </c>
-      <c r="P93" s="48" t="s">
+      <c r="P93" s="47" t="s">
         <v>1064</v>
       </c>
-      <c r="Q93" s="48" t="s">
+      <c r="Q93" s="47" t="s">
         <v>1065</v>
       </c>
-      <c r="R93" s="48" t="s">
+      <c r="R93" s="47" t="s">
         <v>1066</v>
       </c>
-      <c r="S93" s="48" t="s">
+      <c r="S93" s="47" t="s">
         <v>1067</v>
       </c>
-      <c r="T93" s="48" t="s">
+      <c r="T93" s="47" t="s">
         <v>1068</v>
       </c>
-      <c r="U93" s="48" t="s">
+      <c r="U93" s="47" t="s">
         <v>1069</v>
       </c>
-      <c r="V93" s="48" t="s">
+      <c r="V93" s="47" t="s">
         <v>1070</v>
       </c>
-      <c r="W93" s="48" t="s">
+      <c r="W93" s="47" t="s">
         <v>1071</v>
       </c>
-      <c r="X93" s="48" t="s">
+      <c r="X93" s="47" t="s">
         <v>1072</v>
       </c>
-      <c r="Y93" s="48" t="s">
+      <c r="Y93" s="47" t="s">
         <v>1073</v>
       </c>
-      <c r="Z93" s="48" t="s">
+      <c r="Z93" s="47" t="s">
         <v>1074</v>
       </c>
-      <c r="AA93" s="48" t="s">
+      <c r="AA93" s="47" t="s">
         <v>1075</v>
       </c>
-      <c r="AB93" s="48" t="s">
+      <c r="AB93" s="47" t="s">
         <v>1076</v>
       </c>
-      <c r="AC93" s="48" t="s">
+      <c r="AC93" s="47" t="s">
         <v>1077</v>
       </c>
-      <c r="AD93" s="48" t="s">
+      <c r="AD93" s="47" t="s">
         <v>1078</v>
       </c>
-      <c r="AE93" s="48" t="s">
+      <c r="AE93" s="47" t="s">
         <v>1079</v>
       </c>
-      <c r="AF93" s="48" t="s">
+      <c r="AF93" s="47" t="s">
         <v>1080</v>
       </c>
     </row>
     <row r="94" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B94" s="47" t="s">
+      <c r="B94" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="C94" s="49">
+      <c r="C94" s="48">
         <v>169.071</v>
       </c>
-      <c r="D94" s="49">
+      <c r="D94" s="48">
         <v>175.941</v>
       </c>
-      <c r="E94" s="49">
+      <c r="E94" s="48">
         <v>182.26900000000001</v>
       </c>
-      <c r="F94" s="49">
+      <c r="F94" s="48">
         <v>183.286</v>
       </c>
-      <c r="G94" s="49">
+      <c r="G94" s="48">
         <v>180.57400000000001</v>
       </c>
-      <c r="H94" s="49">
+      <c r="H94" s="48">
         <v>172.66399999999999</v>
       </c>
-      <c r="I94" s="49">
+      <c r="I94" s="48">
         <v>163.08199999999999</v>
       </c>
-      <c r="J94" s="49">
+      <c r="J94" s="48">
         <v>147.75899999999999</v>
       </c>
-      <c r="K94" s="49">
+      <c r="K94" s="48">
         <v>115.26</v>
       </c>
-      <c r="L94" s="49">
+      <c r="L94" s="48">
         <v>111.494</v>
       </c>
-      <c r="M94" s="49">
+      <c r="M94" s="48">
         <v>104.2</v>
       </c>
-      <c r="N94" s="49">
+      <c r="N94" s="48">
         <v>97.091999999999999</v>
       </c>
-      <c r="O94" s="49">
+      <c r="O94" s="48">
         <v>86.153000000000006</v>
       </c>
-      <c r="P94" s="49">
+      <c r="P94" s="48">
         <v>75.078000000000003</v>
       </c>
-      <c r="Q94" s="49">
+      <c r="Q94" s="48">
         <v>69.908000000000001</v>
       </c>
-      <c r="R94" s="49">
+      <c r="R94" s="48">
         <v>65.022000000000006</v>
       </c>
-      <c r="S94" s="49">
+      <c r="S94" s="48">
         <v>60.552999999999997</v>
       </c>
-      <c r="T94" s="49">
+      <c r="T94" s="48">
         <v>56.177</v>
       </c>
-      <c r="U94" s="49">
+      <c r="U94" s="48">
         <v>52.183</v>
       </c>
-      <c r="V94" s="49">
+      <c r="V94" s="48">
         <v>48.268000000000001</v>
       </c>
-      <c r="W94" s="49">
+      <c r="W94" s="48">
         <v>44.52</v>
       </c>
-      <c r="X94" s="49">
+      <c r="X94" s="48">
         <v>40.801000000000002</v>
       </c>
-      <c r="Y94" s="49">
+      <c r="Y94" s="48">
         <v>37.277000000000001</v>
       </c>
-      <c r="Z94" s="49">
+      <c r="Z94" s="48">
         <v>33.844999999999999</v>
       </c>
-      <c r="AA94" s="49">
+      <c r="AA94" s="48">
         <v>30.599</v>
       </c>
-      <c r="AB94" s="49">
+      <c r="AB94" s="48">
         <v>27.539000000000001</v>
       </c>
-      <c r="AC94" s="49">
+      <c r="AC94" s="48">
         <v>24.655000000000001</v>
       </c>
-      <c r="AD94" s="49">
+      <c r="AD94" s="48">
         <v>22.006</v>
       </c>
-      <c r="AE94" s="49">
+      <c r="AE94" s="48">
         <v>19.544</v>
       </c>
-      <c r="AF94" s="49">
+      <c r="AF94" s="48">
         <v>17.234999999999999</v>
       </c>
     </row>
     <row r="95" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B95" s="47" t="s">
+      <c r="B95" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="C95" s="49">
+      <c r="C95" s="48">
         <v>351.60700000000003</v>
       </c>
-      <c r="D95" s="49">
+      <c r="D95" s="48">
         <v>365.89499999999998</v>
       </c>
-      <c r="E95" s="49">
+      <c r="E95" s="48">
         <v>379.05500000000001</v>
       </c>
-      <c r="F95" s="49">
+      <c r="F95" s="48">
         <v>381.17</v>
       </c>
-      <c r="G95" s="49">
+      <c r="G95" s="48">
         <v>375.53</v>
       </c>
-      <c r="H95" s="49">
+      <c r="H95" s="48">
         <v>359.08</v>
       </c>
-      <c r="I95" s="49">
+      <c r="I95" s="48">
         <v>339.15199999999999</v>
       </c>
-      <c r="J95" s="49">
+      <c r="J95" s="48">
         <v>307.286</v>
       </c>
-      <c r="K95" s="49">
+      <c r="K95" s="48">
         <v>268.94</v>
       </c>
-      <c r="L95" s="49">
+      <c r="L95" s="48">
         <v>260.65199999999999</v>
       </c>
-      <c r="M95" s="49">
+      <c r="M95" s="48">
         <v>243.6</v>
       </c>
-      <c r="N95" s="49">
+      <c r="N95" s="48">
         <v>227.10599999999999</v>
       </c>
-      <c r="O95" s="49">
+      <c r="O95" s="48">
         <v>201.94499999999999</v>
       </c>
-      <c r="P95" s="49">
+      <c r="P95" s="48">
         <v>176.53700000000001</v>
       </c>
-      <c r="Q95" s="49">
+      <c r="Q95" s="48">
         <v>165.084</v>
       </c>
-      <c r="R95" s="49">
+      <c r="R95" s="48">
         <v>154.726</v>
       </c>
-      <c r="S95" s="49">
+      <c r="S95" s="48">
         <v>145.71299999999999</v>
       </c>
-      <c r="T95" s="49">
+      <c r="T95" s="48">
         <v>137.16499999999999</v>
       </c>
-      <c r="U95" s="49">
+      <c r="U95" s="48">
         <v>129.738</v>
       </c>
-      <c r="V95" s="49">
+      <c r="V95" s="48">
         <v>122.61199999999999</v>
       </c>
-      <c r="W95" s="49">
+      <c r="W95" s="48">
         <v>115.96899999999999</v>
       </c>
-      <c r="X95" s="49">
+      <c r="X95" s="48">
         <v>109.38</v>
       </c>
-      <c r="Y95" s="49">
+      <c r="Y95" s="48">
         <v>103.21299999999999</v>
       </c>
-      <c r="Z95" s="49">
+      <c r="Z95" s="48">
         <v>97.149000000000001</v>
       </c>
-      <c r="AA95" s="49">
+      <c r="AA95" s="48">
         <v>91.388000000000005</v>
       </c>
-      <c r="AB95" s="49">
+      <c r="AB95" s="48">
         <v>85.896000000000001</v>
       </c>
-      <c r="AC95" s="49">
+      <c r="AC95" s="48">
         <v>80.599000000000004</v>
       </c>
-      <c r="AD95" s="49">
+      <c r="AD95" s="48">
         <v>75.680999999999997</v>
       </c>
-      <c r="AE95" s="49">
+      <c r="AE95" s="48">
         <v>70.977999999999994</v>
       </c>
-      <c r="AF95" s="49">
+      <c r="AF95" s="48">
         <v>66.334999999999994</v>
       </c>
     </row>
     <row r="96" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B96" s="47" t="s">
+      <c r="B96" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="C96" s="49">
+      <c r="C96" s="48">
         <v>338.14100000000002</v>
       </c>
-      <c r="D96" s="49">
+      <c r="D96" s="48">
         <v>351.88200000000001</v>
       </c>
-      <c r="E96" s="49">
+      <c r="E96" s="48">
         <v>364.53800000000001</v>
       </c>
-      <c r="F96" s="49">
+      <c r="F96" s="48">
         <v>366.572</v>
       </c>
-      <c r="G96" s="49">
+      <c r="G96" s="48">
         <v>361.14800000000002</v>
       </c>
-      <c r="H96" s="49">
+      <c r="H96" s="48">
         <v>345.32799999999997</v>
       </c>
-      <c r="I96" s="49">
+      <c r="I96" s="48">
         <v>326.16300000000001</v>
       </c>
-      <c r="J96" s="49">
+      <c r="J96" s="48">
         <v>295.517</v>
       </c>
-      <c r="K96" s="49">
+      <c r="K96" s="48">
         <v>251.99</v>
       </c>
-      <c r="L96" s="49">
+      <c r="L96" s="48">
         <v>253.26900000000001</v>
       </c>
-      <c r="M96" s="49">
+      <c r="M96" s="48">
         <v>236.7</v>
       </c>
-      <c r="N96" s="49">
+      <c r="N96" s="48">
         <v>221.43299999999999</v>
       </c>
-      <c r="O96" s="49">
+      <c r="O96" s="48">
         <v>202.35</v>
       </c>
-      <c r="P96" s="49">
+      <c r="P96" s="48">
         <v>179.768</v>
       </c>
-      <c r="Q96" s="49">
+      <c r="Q96" s="48">
         <v>171.83699999999999</v>
       </c>
-      <c r="R96" s="49">
+      <c r="R96" s="48">
         <v>164.82400000000001</v>
       </c>
-      <c r="S96" s="49">
+      <c r="S96" s="48">
         <v>159.05699999999999</v>
       </c>
-      <c r="T96" s="49">
+      <c r="T96" s="48">
         <v>153.62100000000001</v>
       </c>
-      <c r="U96" s="49">
+      <c r="U96" s="48">
         <v>149.28700000000001</v>
       </c>
-      <c r="V96" s="49">
+      <c r="V96" s="48">
         <v>145.18</v>
       </c>
-      <c r="W96" s="49">
+      <c r="W96" s="48">
         <v>141.511</v>
       </c>
-      <c r="X96" s="49">
+      <c r="X96" s="48">
         <v>137.78299999999999</v>
       </c>
-      <c r="Y96" s="49">
+      <c r="Y96" s="48">
         <v>134.44999999999999</v>
       </c>
-      <c r="Z96" s="49">
+      <c r="Z96" s="48">
         <v>131.119</v>
       </c>
-      <c r="AA96" s="49">
+      <c r="AA96" s="48">
         <v>128.054</v>
       </c>
-      <c r="AB96" s="49">
+      <c r="AB96" s="48">
         <v>125.217</v>
       </c>
-      <c r="AC96" s="49">
+      <c r="AC96" s="48">
         <v>122.514</v>
       </c>
-      <c r="AD96" s="49">
+      <c r="AD96" s="48">
         <v>120.251</v>
       </c>
-      <c r="AE96" s="49">
+      <c r="AE96" s="48">
         <v>118.178</v>
       </c>
-      <c r="AF96" s="49">
+      <c r="AF96" s="48">
         <v>116.047</v>
       </c>
     </row>
     <row r="97" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B97" s="47" t="s">
+      <c r="B97" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="C97" s="49">
+      <c r="C97" s="48">
         <v>284.27800000000002</v>
       </c>
-      <c r="D97" s="49">
+      <c r="D97" s="48">
         <v>295.83</v>
       </c>
-      <c r="E97" s="49">
+      <c r="E97" s="48">
         <v>306.47000000000003</v>
       </c>
-      <c r="F97" s="49">
+      <c r="F97" s="48">
         <v>308.18</v>
       </c>
-      <c r="G97" s="49">
+      <c r="G97" s="48">
         <v>303.62</v>
       </c>
-      <c r="H97" s="49">
+      <c r="H97" s="48">
         <v>290.32</v>
       </c>
-      <c r="I97" s="49">
+      <c r="I97" s="48">
         <v>274.20800000000003</v>
       </c>
-      <c r="J97" s="49">
+      <c r="J97" s="48">
         <v>248.44399999999999</v>
       </c>
-      <c r="K97" s="49">
+      <c r="K97" s="48">
         <v>206.79</v>
       </c>
-      <c r="L97" s="49">
+      <c r="L97" s="48">
         <v>196.238</v>
       </c>
-      <c r="M97" s="49">
+      <c r="M97" s="48">
         <v>183.4</v>
       </c>
-      <c r="N97" s="49">
+      <c r="N97" s="48">
         <v>170.56200000000001</v>
       </c>
-      <c r="O97" s="49">
+      <c r="O97" s="48">
         <v>149.16399999999999</v>
       </c>
-      <c r="P97" s="49">
+      <c r="P97" s="48">
         <v>129.59200000000001</v>
       </c>
-      <c r="Q97" s="49">
+      <c r="Q97" s="48">
         <v>120.236</v>
       </c>
-      <c r="R97" s="49">
+      <c r="R97" s="48">
         <v>112.6</v>
       </c>
-      <c r="S97" s="49">
+      <c r="S97" s="48">
         <v>106.702</v>
       </c>
-      <c r="T97" s="49">
+      <c r="T97" s="48">
         <v>101.782</v>
       </c>
-      <c r="U97" s="49">
+      <c r="U97" s="48">
         <v>98.244</v>
       </c>
-      <c r="V97" s="49">
+      <c r="V97" s="48">
         <v>95.421000000000006</v>
       </c>
-      <c r="W97" s="49">
+      <c r="W97" s="48">
         <v>93.405000000000001</v>
       </c>
-      <c r="X97" s="49">
+      <c r="X97" s="48">
         <v>91.822999999999993</v>
       </c>
-      <c r="Y97" s="49">
+      <c r="Y97" s="48">
         <v>90.944999999999993</v>
       </c>
-      <c r="Z97" s="49">
+      <c r="Z97" s="48">
         <v>90.488</v>
       </c>
-      <c r="AA97" s="49">
+      <c r="AA97" s="48">
         <v>90.611000000000004</v>
       </c>
-      <c r="AB97" s="49">
+      <c r="AB97" s="48">
         <v>91.287999999999997</v>
       </c>
-      <c r="AC97" s="49">
+      <c r="AC97" s="48">
         <v>92.462000000000003</v>
       </c>
-      <c r="AD97" s="49">
+      <c r="AD97" s="48">
         <v>94.373000000000005</v>
       </c>
-      <c r="AE97" s="49">
+      <c r="AE97" s="48">
         <v>96.867000000000004</v>
       </c>
-      <c r="AF97" s="49">
+      <c r="AF97" s="48">
         <v>99.762</v>
       </c>
     </row>
     <row r="98" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B98" s="47" t="s">
+      <c r="B98" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="C98" s="49">
+      <c r="C98" s="48">
         <v>203.483</v>
       </c>
-      <c r="D98" s="49">
+      <c r="D98" s="48">
         <v>211.75200000000001</v>
       </c>
-      <c r="E98" s="49">
+      <c r="E98" s="48">
         <v>219.36799999999999</v>
       </c>
-      <c r="F98" s="49">
+      <c r="F98" s="48">
         <v>220.59200000000001</v>
       </c>
-      <c r="G98" s="49">
+      <c r="G98" s="48">
         <v>217.328</v>
       </c>
-      <c r="H98" s="49">
+      <c r="H98" s="48">
         <v>207.80799999999999</v>
       </c>
-      <c r="I98" s="49">
+      <c r="I98" s="48">
         <v>196.27500000000001</v>
       </c>
-      <c r="J98" s="49">
+      <c r="J98" s="48">
         <v>177.834</v>
       </c>
-      <c r="K98" s="49">
+      <c r="K98" s="48">
         <v>161.59</v>
       </c>
-      <c r="L98" s="49">
+      <c r="L98" s="48">
         <v>143.273</v>
       </c>
-      <c r="M98" s="49">
+      <c r="M98" s="48">
         <v>133.9</v>
       </c>
-      <c r="N98" s="49">
+      <c r="N98" s="48">
         <v>123.69</v>
       </c>
-      <c r="O98" s="49">
+      <c r="O98" s="48">
         <v>102.069</v>
       </c>
-      <c r="P98" s="49">
+      <c r="P98" s="48">
         <v>85.85</v>
       </c>
-      <c r="Q98" s="49">
+      <c r="Q98" s="48">
         <v>76.216999999999999</v>
       </c>
-      <c r="R98" s="49">
+      <c r="R98" s="48">
         <v>68.501999999999995</v>
       </c>
-      <c r="S98" s="49">
+      <c r="S98" s="48">
         <v>62.488</v>
       </c>
-      <c r="T98" s="49">
+      <c r="T98" s="48">
         <v>57.558999999999997</v>
       </c>
-      <c r="U98" s="49">
+      <c r="U98" s="48">
         <v>53.819000000000003</v>
       </c>
-      <c r="V98" s="49">
+      <c r="V98" s="48">
         <v>50.801000000000002</v>
       </c>
-      <c r="W98" s="49">
+      <c r="W98" s="48">
         <v>48.494</v>
       </c>
-      <c r="X98" s="49">
+      <c r="X98" s="48">
         <v>46.64</v>
       </c>
-      <c r="Y98" s="49">
+      <c r="Y98" s="48">
         <v>45.348999999999997</v>
       </c>
-      <c r="Z98" s="49">
+      <c r="Z98" s="48">
         <v>44.445999999999998</v>
       </c>
-      <c r="AA98" s="49">
+      <c r="AA98" s="48">
         <v>43.994999999999997</v>
       </c>
-      <c r="AB98" s="49">
+      <c r="AB98" s="48">
         <v>43.973999999999997</v>
       </c>
-      <c r="AC98" s="49">
+      <c r="AC98" s="48">
         <v>44.338000000000001</v>
       </c>
-      <c r="AD98" s="49">
+      <c r="AD98" s="48">
         <v>45.216000000000001</v>
       </c>
-      <c r="AE98" s="49">
+      <c r="AE98" s="48">
         <v>46.536999999999999</v>
       </c>
-      <c r="AF98" s="49">
+      <c r="AF98" s="48">
         <v>48.232999999999997</v>
       </c>
     </row>
     <row r="99" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B99" s="47" t="s">
+      <c r="B99" s="46" t="s">
         <v>142</v>
       </c>
-      <c r="C99" s="49">
+      <c r="C99" s="48">
         <v>110.71899999999999</v>
       </c>
-      <c r="D99" s="49">
+      <c r="D99" s="48">
         <v>115.218</v>
       </c>
-      <c r="E99" s="49">
+      <c r="E99" s="48">
         <v>119.36199999999999</v>
       </c>
-      <c r="F99" s="49">
+      <c r="F99" s="48">
         <v>120.02800000000001</v>
       </c>
-      <c r="G99" s="49">
+      <c r="G99" s="48">
         <v>118.252</v>
       </c>
-      <c r="H99" s="49">
+      <c r="H99" s="48">
         <v>113.072</v>
       </c>
-      <c r="I99" s="49">
+      <c r="I99" s="48">
         <v>106.797</v>
       </c>
-      <c r="J99" s="49">
+      <c r="J99" s="48">
         <v>96.762</v>
       </c>
-      <c r="K99" s="49">
+      <c r="K99" s="48">
         <v>73.45</v>
       </c>
-      <c r="L99" s="49">
+      <c r="L99" s="48">
         <v>62.381</v>
       </c>
-      <c r="M99" s="49">
+      <c r="M99" s="48">
         <v>58.3</v>
       </c>
-      <c r="N99" s="49">
+      <c r="N99" s="48">
         <v>53.567999999999998</v>
       </c>
-      <c r="O99" s="49">
+      <c r="O99" s="48">
         <v>42.386000000000003</v>
       </c>
-      <c r="P99" s="49">
+      <c r="P99" s="48">
         <v>34.78</v>
       </c>
-      <c r="Q99" s="49">
+      <c r="Q99" s="48">
         <v>29.864000000000001</v>
       </c>
-      <c r="R99" s="49">
+      <c r="R99" s="48">
         <v>25.962</v>
       </c>
-      <c r="S99" s="49">
+      <c r="S99" s="48">
         <v>22.911000000000001</v>
       </c>
-      <c r="T99" s="49">
+      <c r="T99" s="48">
         <v>20.411999999999999</v>
       </c>
-      <c r="U99" s="49">
+      <c r="U99" s="48">
         <v>18.466000000000001</v>
       </c>
-      <c r="V99" s="49">
+      <c r="V99" s="48">
         <v>16.864000000000001</v>
       </c>
-      <c r="W99" s="49">
+      <c r="W99" s="48">
         <v>15.573</v>
       </c>
-      <c r="X99" s="49">
+      <c r="X99" s="48">
         <v>14.496</v>
       </c>
-      <c r="Y99" s="49">
+      <c r="Y99" s="48">
         <v>13.64</v>
       </c>
-      <c r="Z99" s="49">
+      <c r="Z99" s="48">
         <v>12.938000000000001</v>
       </c>
-      <c r="AA99" s="49">
+      <c r="AA99" s="48">
         <v>12.398</v>
       </c>
-      <c r="AB99" s="49">
+      <c r="AB99" s="48">
         <v>11.999000000000001</v>
       </c>
-      <c r="AC99" s="49">
+      <c r="AC99" s="48">
         <v>11.718999999999999</v>
       </c>
-      <c r="AD99" s="49">
+      <c r="AD99" s="48">
         <v>11.583</v>
       </c>
-      <c r="AE99" s="49">
+      <c r="AE99" s="48">
         <v>11.557</v>
       </c>
-      <c r="AF99" s="49">
+      <c r="AF99" s="48">
         <v>11.621</v>
       </c>
     </row>
     <row r="100" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B100" s="47" t="s">
+      <c r="B100" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="C100" s="49">
+      <c r="C100" s="48">
         <v>38.901000000000003</v>
       </c>
-      <c r="D100" s="49">
+      <c r="D100" s="48">
         <v>40.481999999999999</v>
       </c>
-      <c r="E100" s="49">
+      <c r="E100" s="48">
         <v>41.938000000000002</v>
       </c>
-      <c r="F100" s="49">
+      <c r="F100" s="48">
         <v>42.171999999999997</v>
       </c>
-      <c r="G100" s="49">
+      <c r="G100" s="48">
         <v>41.548000000000002</v>
       </c>
-      <c r="H100" s="49">
+      <c r="H100" s="48">
         <v>39.728000000000002</v>
       </c>
-      <c r="I100" s="49">
+      <c r="I100" s="48">
         <v>37.523000000000003</v>
       </c>
-      <c r="J100" s="49">
+      <c r="J100" s="48">
         <v>33.997999999999998</v>
       </c>
-      <c r="K100" s="49">
+      <c r="K100" s="48">
         <v>51.98</v>
       </c>
-      <c r="L100" s="49">
+      <c r="L100" s="48">
         <v>42.692999999999998</v>
       </c>
-      <c r="M100" s="49">
+      <c r="M100" s="48">
         <v>39.9</v>
       </c>
-      <c r="N100" s="49">
+      <c r="N100" s="48">
         <v>36.548999999999999</v>
       </c>
-      <c r="O100" s="49">
+      <c r="O100" s="48">
         <v>27.933</v>
       </c>
-      <c r="P100" s="49">
+      <c r="P100" s="48">
         <v>22.395</v>
       </c>
-      <c r="Q100" s="49">
+      <c r="Q100" s="48">
         <v>18.614000000000001</v>
       </c>
-      <c r="R100" s="49">
+      <c r="R100" s="48">
         <v>15.544</v>
       </c>
-      <c r="S100" s="49">
+      <c r="S100" s="48">
         <v>13.076000000000001</v>
       </c>
-      <c r="T100" s="49">
+      <c r="T100" s="48">
         <v>11.023999999999999</v>
       </c>
-      <c r="U100" s="49">
+      <c r="U100" s="48">
         <v>9.3629999999999995</v>
       </c>
-      <c r="V100" s="49">
+      <c r="V100" s="48">
         <v>7.9740000000000002</v>
       </c>
-      <c r="W100" s="49">
+      <c r="W100" s="48">
         <v>6.8079999999999998</v>
       </c>
-      <c r="X100" s="49">
+      <c r="X100" s="48">
         <v>5.8170000000000002</v>
       </c>
-      <c r="Y100" s="49">
+      <c r="Y100" s="48">
         <v>4.9859999999999998</v>
       </c>
-      <c r="Z100" s="49">
+      <c r="Z100" s="48">
         <v>4.2750000000000004</v>
       </c>
-      <c r="AA100" s="49">
+      <c r="AA100" s="48">
         <v>3.6749999999999998</v>
       </c>
-      <c r="AB100" s="49">
+      <c r="AB100" s="48">
         <v>3.1669999999999998</v>
       </c>
-      <c r="AC100" s="49">
+      <c r="AC100" s="48">
         <v>2.7330000000000001</v>
       </c>
-      <c r="AD100" s="49">
+      <c r="AD100" s="48">
         <v>2.37</v>
       </c>
-      <c r="AE100" s="49">
+      <c r="AE100" s="48">
         <v>2.0590000000000002</v>
       </c>
-      <c r="AF100" s="49">
+      <c r="AF100" s="48">
         <v>1.7869999999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B102" s="37" t="s">
+        <v>340</v>
+      </c>
+      <c r="C102" s="37"/>
+      <c r="D102" s="37"/>
+      <c r="E102" s="37"/>
+      <c r="F102" s="37"/>
+      <c r="G102" s="37"/>
+      <c r="H102" s="37"/>
+      <c r="I102" s="37"/>
+    </row>
+    <row r="103" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B103" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C103" s="37" t="s">
+        <v>342</v>
+      </c>
+      <c r="D103" s="37" t="s">
+        <v>1085</v>
+      </c>
+      <c r="E103" s="37" t="s">
+        <v>456</v>
+      </c>
+      <c r="F103" s="37" t="s">
+        <v>457</v>
+      </c>
+      <c r="G103" s="37" t="s">
+        <v>458</v>
+      </c>
+      <c r="H103" s="37" t="s">
+        <v>459</v>
+      </c>
+      <c r="I103" s="37" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="104" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B104" s="37" t="s">
+        <v>462</v>
+      </c>
+      <c r="C104" s="20">
+        <v>0</v>
+      </c>
+      <c r="D104" s="20">
+        <v>0</v>
+      </c>
+      <c r="E104" s="20">
+        <f>D104*K$52</f>
+        <v>0</v>
+      </c>
+      <c r="F104" s="20">
+        <f>D104*L$52</f>
+        <v>0</v>
+      </c>
+      <c r="G104" s="20">
+        <f>D104*M$52</f>
+        <v>0</v>
+      </c>
+      <c r="H104" s="20">
+        <f>D104*N$52</f>
+        <v>0</v>
+      </c>
+      <c r="I104" s="20">
+        <f>D104*O$52</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B105" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="C105" s="20">
+        <v>0</v>
+      </c>
+      <c r="D105" s="20">
+        <v>0</v>
+      </c>
+      <c r="E105" s="20">
+        <f t="shared" ref="E105:E119" si="17">D105*K$52</f>
+        <v>0</v>
+      </c>
+      <c r="F105" s="20">
+        <f t="shared" ref="F105:F119" si="18">D105*L$52</f>
+        <v>0</v>
+      </c>
+      <c r="G105" s="20">
+        <f t="shared" ref="G105:G119" si="19">D105*M$52</f>
+        <v>0</v>
+      </c>
+      <c r="H105" s="20">
+        <f t="shared" ref="H105:H119" si="20">D105*N$52</f>
+        <v>0</v>
+      </c>
+      <c r="I105" s="20">
+        <f t="shared" ref="I105:I119" si="21">D105*O$52</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B106" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="C106" s="37">
+        <v>0</v>
+      </c>
+      <c r="D106" s="37">
+        <f>C106/1000</f>
+        <v>0</v>
+      </c>
+      <c r="E106" s="20">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F106" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G106" s="20">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H106" s="20">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I106" s="20">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B107" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="C107" s="37">
+        <v>179</v>
+      </c>
+      <c r="D107" s="52">
+        <f>183.286/1000</f>
+        <v>0.183286</v>
+      </c>
+      <c r="E107" s="20">
+        <f t="shared" si="17"/>
+        <v>0.183286</v>
+      </c>
+      <c r="F107" s="20">
+        <f t="shared" si="18"/>
+        <v>0.183286</v>
+      </c>
+      <c r="G107" s="20">
+        <f t="shared" si="19"/>
+        <v>0.10630587999999999</v>
+      </c>
+      <c r="H107" s="20">
+        <f t="shared" si="20"/>
+        <v>0.10630587999999999</v>
+      </c>
+      <c r="I107" s="20">
+        <f t="shared" si="21"/>
+        <v>7.5147259999999994E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B108" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="C108" s="37">
+        <v>368</v>
+      </c>
+      <c r="D108" s="52">
+        <f>381.17/1000</f>
+        <v>0.38117000000000001</v>
+      </c>
+      <c r="E108" s="20">
+        <f t="shared" si="17"/>
+        <v>0.38117000000000001</v>
+      </c>
+      <c r="F108" s="20">
+        <f t="shared" si="18"/>
+        <v>0.38117000000000001</v>
+      </c>
+      <c r="G108" s="20">
+        <f t="shared" si="19"/>
+        <v>0.22107859999999999</v>
+      </c>
+      <c r="H108" s="20">
+        <f t="shared" si="20"/>
+        <v>0.22107859999999999</v>
+      </c>
+      <c r="I108" s="20">
+        <f t="shared" si="21"/>
+        <v>0.15627969999999999</v>
+      </c>
+    </row>
+    <row r="109" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B109" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="C109" s="37">
+        <v>372</v>
+      </c>
+      <c r="D109" s="52">
+        <f>366.572/1000</f>
+        <v>0.36657200000000001</v>
+      </c>
+      <c r="E109" s="20">
+        <f t="shared" si="17"/>
+        <v>0.36657200000000001</v>
+      </c>
+      <c r="F109" s="20">
+        <f t="shared" si="18"/>
+        <v>0.36657200000000001</v>
+      </c>
+      <c r="G109" s="20">
+        <f t="shared" si="19"/>
+        <v>0.21261175999999998</v>
+      </c>
+      <c r="H109" s="20">
+        <f t="shared" si="20"/>
+        <v>0.21261175999999998</v>
+      </c>
+      <c r="I109" s="20">
+        <f t="shared" si="21"/>
+        <v>0.15029451999999999</v>
+      </c>
+    </row>
+    <row r="110" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B110" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="C110" s="37">
+        <v>311</v>
+      </c>
+      <c r="D110" s="52">
+        <f>308.18/1000</f>
+        <v>0.30818000000000001</v>
+      </c>
+      <c r="E110" s="20">
+        <f t="shared" si="17"/>
+        <v>0.30818000000000001</v>
+      </c>
+      <c r="F110" s="20">
+        <f t="shared" si="18"/>
+        <v>0.30818000000000001</v>
+      </c>
+      <c r="G110" s="20">
+        <f t="shared" si="19"/>
+        <v>0.1787444</v>
+      </c>
+      <c r="H110" s="20">
+        <f t="shared" si="20"/>
+        <v>0.1787444</v>
+      </c>
+      <c r="I110" s="20">
+        <f t="shared" si="21"/>
+        <v>0.12635379999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B111" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="C111" s="37">
+        <v>226</v>
+      </c>
+      <c r="D111" s="52">
+        <f>220.592/1000</f>
+        <v>0.22059200000000001</v>
+      </c>
+      <c r="E111" s="20">
+        <f t="shared" si="17"/>
+        <v>0.22059200000000001</v>
+      </c>
+      <c r="F111" s="20">
+        <f t="shared" si="18"/>
+        <v>0.22059200000000001</v>
+      </c>
+      <c r="G111" s="20">
+        <f t="shared" si="19"/>
+        <v>0.12794336000000001</v>
+      </c>
+      <c r="H111" s="20">
+        <f t="shared" si="20"/>
+        <v>0.12794336000000001</v>
+      </c>
+      <c r="I111" s="20">
+        <f t="shared" si="21"/>
+        <v>9.0442720000000004E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B112" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="C112" s="37">
+        <v>105</v>
+      </c>
+      <c r="D112" s="52">
+        <f>120.028/1000</f>
+        <v>0.12002800000000001</v>
+      </c>
+      <c r="E112" s="20">
+        <f t="shared" si="17"/>
+        <v>0.12002800000000001</v>
+      </c>
+      <c r="F112" s="20">
+        <f t="shared" si="18"/>
+        <v>0.12002800000000001</v>
+      </c>
+      <c r="G112" s="20">
+        <f t="shared" si="19"/>
+        <v>6.9616239999999996E-2</v>
+      </c>
+      <c r="H112" s="20">
+        <f t="shared" si="20"/>
+        <v>6.9616239999999996E-2</v>
+      </c>
+      <c r="I112" s="20">
+        <f t="shared" si="21"/>
+        <v>4.9211480000000002E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B113" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="C113" s="37">
+        <v>14</v>
+      </c>
+      <c r="D113" s="52">
+        <f>42.172/1000</f>
+        <v>4.2171999999999994E-2</v>
+      </c>
+      <c r="E113" s="20">
+        <f t="shared" si="17"/>
+        <v>4.2171999999999994E-2</v>
+      </c>
+      <c r="F113" s="20">
+        <f t="shared" si="18"/>
+        <v>4.2171999999999994E-2</v>
+      </c>
+      <c r="G113" s="20">
+        <f t="shared" si="19"/>
+        <v>2.4459759999999994E-2</v>
+      </c>
+      <c r="H113" s="20">
+        <f t="shared" si="20"/>
+        <v>2.4459759999999994E-2</v>
+      </c>
+      <c r="I113" s="20">
+        <f t="shared" si="21"/>
+        <v>1.7290519999999997E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B114" s="37" t="s">
+        <v>464</v>
+      </c>
+      <c r="C114" s="20">
+        <v>0</v>
+      </c>
+      <c r="D114" s="20">
+        <v>0</v>
+      </c>
+      <c r="E114" s="20">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F114" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G114" s="20">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H114" s="20">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I114" s="20">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B115" s="37" t="s">
+        <v>465</v>
+      </c>
+      <c r="C115" s="20">
+        <v>0</v>
+      </c>
+      <c r="D115" s="20">
+        <v>0</v>
+      </c>
+      <c r="E115" s="20">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F115" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G115" s="20">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H115" s="20">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I115" s="20">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B116" s="37" t="s">
+        <v>327</v>
+      </c>
+      <c r="C116" s="20">
+        <v>0</v>
+      </c>
+      <c r="D116" s="20">
+        <v>0</v>
+      </c>
+      <c r="E116" s="20">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F116" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G116" s="20">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H116" s="20">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I116" s="20">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B117" s="37" t="s">
+        <v>466</v>
+      </c>
+      <c r="C117" s="20">
+        <v>0</v>
+      </c>
+      <c r="D117" s="20">
+        <v>0</v>
+      </c>
+      <c r="E117" s="20">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F117" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G117" s="20">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H117" s="20">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I117" s="20">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B118" s="37" t="s">
+        <v>467</v>
+      </c>
+      <c r="C118" s="20">
+        <v>0</v>
+      </c>
+      <c r="D118" s="20">
+        <v>0</v>
+      </c>
+      <c r="E118" s="20">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F118" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G118" s="20">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H118" s="20">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I118" s="20">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B119" s="37" t="s">
+        <v>468</v>
+      </c>
+      <c r="C119" s="20">
+        <v>0</v>
+      </c>
+      <c r="D119" s="20">
+        <v>0</v>
+      </c>
+      <c r="E119" s="20">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="F119" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="G119" s="20">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H119" s="20">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I119" s="20">
+        <f t="shared" si="21"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>